<commit_message>
Added ids to Atlanta data, ids to php pull, scores to ATL crimes
</commit_message>
<xml_diff>
--- a/database/General Data/GeneralizedData.xlsx
+++ b/database/General Data/GeneralizedData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="22240" yWindow="2760" windowWidth="25600" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>LARCENY-FROM VEHICLE</t>
   </si>
   <si>
-    <t>LARCENY-NONE VEHICLE</t>
-  </si>
-  <si>
     <t>RAPE</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>CHI Score</t>
+  </si>
+  <si>
+    <t>LARCENY-NON VEHICLE</t>
   </si>
 </sst>
 </file>
@@ -349,8 +349,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -363,11 +395,43 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -699,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -715,126 +779,156 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>0.25</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>0.25</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
@@ -842,122 +936,125 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="3:5">
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="3:5">
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="3:5">
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="3:5">
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="3:5">
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="3:5">
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="3:5">
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="3:5">
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="3:5">
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="3:5">
       <c r="E26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -987,51 +1084,51 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1039,7 +1136,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1047,7 +1144,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1055,7 +1152,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1063,7 +1160,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1071,7 +1168,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -1079,7 +1176,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -1087,7 +1184,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1095,7 +1192,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13">
         <v>999</v>
@@ -1103,7 +1200,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>999</v>
@@ -1111,7 +1208,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>999</v>
@@ -1119,7 +1216,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>999</v>
@@ -1127,7 +1224,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>999</v>
@@ -1135,7 +1232,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>999</v>
@@ -1143,7 +1240,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>999</v>
@@ -1151,7 +1248,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20">
         <v>999</v>
@@ -1159,7 +1256,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <v>999</v>
@@ -1167,7 +1264,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22">
         <v>999</v>

</xml_diff>